<commit_message>
2024.7.31 UPDATED Bearing-diagnostic & stockforecasting
</commit_message>
<xml_diff>
--- a/stockforecasting/300446_history.xlsx
+++ b/stockforecasting/300446_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2176"/>
+  <dimension ref="A1:K2178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -80965,6 +80965,80 @@
         <v>5.02</v>
       </c>
     </row>
+    <row r="2177">
+      <c r="A2177" t="inlineStr">
+        <is>
+          <t>2024-07-29</t>
+        </is>
+      </c>
+      <c r="B2177" t="n">
+        <v>12.99</v>
+      </c>
+      <c r="C2177" t="n">
+        <v>13.03</v>
+      </c>
+      <c r="D2177" t="n">
+        <v>13.18</v>
+      </c>
+      <c r="E2177" t="n">
+        <v>12.94</v>
+      </c>
+      <c r="F2177" t="n">
+        <v>154300</v>
+      </c>
+      <c r="G2177" t="n">
+        <v>201173.05</v>
+      </c>
+      <c r="H2177" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="I2177" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J2177" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K2177" t="n">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="2178">
+      <c r="A2178" t="inlineStr">
+        <is>
+          <t>2024-07-30</t>
+        </is>
+      </c>
+      <c r="B2178" t="n">
+        <v>12.93</v>
+      </c>
+      <c r="C2178" t="n">
+        <v>12.99</v>
+      </c>
+      <c r="D2178" t="n">
+        <v>13.09</v>
+      </c>
+      <c r="E2178" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="F2178" t="n">
+        <v>153334</v>
+      </c>
+      <c r="G2178" t="n">
+        <v>197853.01</v>
+      </c>
+      <c r="H2178" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="I2178" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="J2178" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="K2178" t="n">
+        <v>4.92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>